<commit_message>
Importing object from Contract
</commit_message>
<xml_diff>
--- a/test/data/contracts.xlsx
+++ b/test/data/contracts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Identificador</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>Gás</t>
+  </si>
+  <si>
+    <t>Objeto</t>
+  </si>
+  <si>
+    <t>Cidade de Magaratiba</t>
   </si>
 </sst>
 </file>
@@ -484,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -500,9 +506,10 @@
     <col min="8" max="8" width="27.75" customWidth="1"/>
     <col min="11" max="11" width="22.375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.125" customWidth="1"/>
+    <col min="13" max="13" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -539,8 +546,11 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -572,7 +582,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -601,7 +611,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -630,7 +640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>250</v>
       </c>
@@ -666,6 +676,9 @@
       </c>
       <c r="L5">
         <v>1792051158</v>
+      </c>
+      <c r="M5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Including the field "currency" on model "contract"
</commit_message>
<xml_diff>
--- a/test/data/contracts.xlsx
+++ b/test/data/contracts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Identificador</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>Cidade de Magaratiba</t>
+  </si>
+  <si>
+    <t>Moeda</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>Dolar</t>
+  </si>
+  <si>
+    <t>Euro</t>
   </si>
 </sst>
 </file>
@@ -490,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -509,7 +521,7 @@
     <col min="13" max="13" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,8 +561,11 @@
       <c r="M1" t="s">
         <v>32</v>
       </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -581,8 +596,11 @@
       <c r="K2" t="s">
         <v>18</v>
       </c>
+      <c r="N2" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -610,8 +628,11 @@
       <c r="K3" t="s">
         <v>23</v>
       </c>
+      <c r="N3" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -639,8 +660,11 @@
       <c r="K4" t="s">
         <v>12</v>
       </c>
+      <c r="N4" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>250</v>
       </c>
@@ -679,6 +703,9 @@
       </c>
       <c r="M5" t="s">
         <v>33</v>
+      </c>
+      <c r="N5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>